<commit_message>
basicals finished, improvements await if time available
</commit_message>
<xml_diff>
--- a/data/xxxll.xlsx
+++ b/data/xxxll.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uneven\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uneven\Desktop\codes\python\api_test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA63B23-A234-4B8E-9463-A8157906B540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8BD90D-3379-458D-BFB5-2F7C030AAE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,6 +48,10 @@
   </si>
   <si>
     <t>数值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -91,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -376,12 +381,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,7 +394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -397,15 +402,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -413,7 +418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>

</xml_diff>